<commit_message>
feat: set folder and notebook to download dataset
</commit_message>
<xml_diff>
--- a/datasets/French_trainset_for_chatbots_dealing_with_usual_requests_on_bank_cards_v1.0.0.xlsx
+++ b/datasets/French_trainset_for_chatbots_dealing_with_usual_requests_on_bank_cards_v1.0.0.xlsx
@@ -1832,14 +1832,14 @@
     <t>DOI</t>
   </si>
   <si>
-    <t>10.5281/zenodo.4769949</t>
+    <t>10.5281/zenodo.5648256</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1866,14 +1866,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1976,12 +1968,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2011,13 +2002,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Cellule liée" xfId="1" builtinId="24"/>
-    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6572,7 +6559,7 @@
       <c r="A5" s="15" t="s">
         <v>540</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>541</v>
       </c>
     </row>
@@ -6609,10 +6596,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: update dataset metadata
</commit_message>
<xml_diff>
--- a/datasets/French_trainset_for_chatbots_dealing_with_usual_requests_on_bank_cards_v1.0.0.xlsx
+++ b/datasets/French_trainset_for_chatbots_dealing_with_usual_requests_on_bank_cards_v1.0.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCHILDEW\Documents\INTERACTIVE-CLUSTERING\r-wnlp-interactive-clustering-publications\_datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCHILDEW\Documents\INTERACTIVE-CLUSTERING\github-interactive-clustering-comparative-study\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -6512,8 +6512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>